<commit_message>
MOSIP-31117:Added the langCode "khm" and assigned the zone "MOR"
Signed-off-by: Yash S <119652212+yashmsonkusare@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/mosip_master/xlsx/zone.xlsx
+++ b/mosip_master/xlsx/zone.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kames\IdeaProjects\mosip-data\mosip_master\xlsx\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yash.mohan\Documents\GitHub\mosip-data\mosip_master\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10219E7B-1F69-4178-BB6A-A2EE54204450}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{386A12A0-DB33-465B-99E9-90F94186CF92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1030" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1036" uniqueCount="201">
   <si>
     <t>lang_code</t>
   </si>
@@ -622,13 +622,22 @@
   </si>
   <si>
     <t>Provincia</t>
+  </si>
+  <si>
+    <t>khm</t>
+  </si>
+  <si>
+    <t>ប្រទេសខ្ញុំ</t>
+  </si>
+  <si>
+    <t>ប្រទេស</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -648,6 +657,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -737,7 +751,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -767,6 +781,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -785,9 +802,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -825,7 +842,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -931,7 +948,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1073,7 +1090,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1081,22 +1098,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H148"/>
+  <dimension ref="A1:H149"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A132" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A149" sqref="A149"/>
+    <sheetView tabSelected="1" topLeftCell="A140" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="G153" sqref="G153"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="17.81640625" customWidth="1"/>
-    <col min="4" max="4" width="16.81640625" customWidth="1"/>
-    <col min="5" max="5" width="23.453125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="19.26953125" customWidth="1"/>
-    <col min="8" max="8" width="8.453125" style="2"/>
+    <col min="3" max="3" width="17.85546875" customWidth="1"/>
+    <col min="4" max="4" width="16.85546875" customWidth="1"/>
+    <col min="5" max="5" width="23.42578125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1122,7 +1139,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>8</v>
       </c>
@@ -1145,7 +1162,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -1168,7 +1185,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>8</v>
       </c>
@@ -1194,7 +1211,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -1220,7 +1237,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
@@ -1246,7 +1263,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>13</v>
       </c>
@@ -1272,7 +1289,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>8</v>
       </c>
@@ -1298,7 +1315,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>13</v>
       </c>
@@ -1324,7 +1341,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1350,7 +1367,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
@@ -1376,7 +1393,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -1402,7 +1419,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>13</v>
       </c>
@@ -1428,7 +1445,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>8</v>
       </c>
@@ -1454,7 +1471,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1480,7 +1497,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>8</v>
       </c>
@@ -1506,7 +1523,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>13</v>
       </c>
@@ -1532,7 +1549,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>8</v>
       </c>
@@ -1558,7 +1575,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>13</v>
       </c>
@@ -1584,7 +1601,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>8</v>
       </c>
@@ -1610,7 +1627,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>13</v>
       </c>
@@ -1636,7 +1653,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>8</v>
       </c>
@@ -1662,7 +1679,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>13</v>
       </c>
@@ -1688,7 +1705,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>8</v>
       </c>
@@ -1714,7 +1731,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>13</v>
       </c>
@@ -1740,7 +1757,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>8</v>
       </c>
@@ -1766,7 +1783,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
         <v>13</v>
       </c>
@@ -1792,7 +1809,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
         <v>8</v>
       </c>
@@ -1818,7 +1835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
         <v>13</v>
       </c>
@@ -1844,7 +1861,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
         <v>8</v>
       </c>
@@ -1870,7 +1887,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
         <v>13</v>
       </c>
@@ -1896,7 +1913,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
         <v>8</v>
       </c>
@@ -1922,7 +1939,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
         <v>13</v>
       </c>
@@ -1948,7 +1965,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
         <v>8</v>
       </c>
@@ -1974,7 +1991,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
         <v>13</v>
       </c>
@@ -2000,7 +2017,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
         <v>8</v>
       </c>
@@ -2026,7 +2043,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
         <v>13</v>
       </c>
@@ -2052,7 +2069,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
         <v>8</v>
       </c>
@@ -2078,7 +2095,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
         <v>13</v>
       </c>
@@ -2104,7 +2121,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
         <v>8</v>
       </c>
@@ -2130,7 +2147,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
         <v>13</v>
       </c>
@@ -2156,7 +2173,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
         <v>8</v>
       </c>
@@ -2182,7 +2199,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
         <v>13</v>
       </c>
@@ -2208,7 +2225,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
         <v>86</v>
       </c>
@@ -2231,7 +2248,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
         <v>86</v>
       </c>
@@ -2257,7 +2274,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
         <v>86</v>
       </c>
@@ -2283,7 +2300,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
         <v>86</v>
       </c>
@@ -2309,7 +2326,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
         <v>86</v>
       </c>
@@ -2335,7 +2352,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
         <v>86</v>
       </c>
@@ -2361,7 +2378,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
         <v>86</v>
       </c>
@@ -2387,7 +2404,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
         <v>86</v>
       </c>
@@ -2413,7 +2430,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
         <v>86</v>
       </c>
@@ -2439,7 +2456,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>86</v>
       </c>
@@ -2465,7 +2482,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>86</v>
       </c>
@@ -2491,7 +2508,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
         <v>86</v>
       </c>
@@ -2517,7 +2534,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
         <v>86</v>
       </c>
@@ -2543,7 +2560,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
         <v>86</v>
       </c>
@@ -2569,7 +2586,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>86</v>
       </c>
@@ -2595,7 +2612,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>86</v>
       </c>
@@ -2621,7 +2638,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
         <v>86</v>
       </c>
@@ -2647,7 +2664,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
         <v>86</v>
       </c>
@@ -2673,7 +2690,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
         <v>86</v>
       </c>
@@ -2699,7 +2716,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
         <v>86</v>
       </c>
@@ -2725,7 +2742,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
         <v>86</v>
       </c>
@@ -2751,7 +2768,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
         <v>112</v>
       </c>
@@ -2774,7 +2791,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
         <v>112</v>
       </c>
@@ -2800,7 +2817,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
         <v>112</v>
       </c>
@@ -2826,7 +2843,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
         <v>112</v>
       </c>
@@ -2852,7 +2869,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
         <v>112</v>
       </c>
@@ -2878,7 +2895,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
         <v>112</v>
       </c>
@@ -2904,7 +2921,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
         <v>112</v>
       </c>
@@ -2930,7 +2947,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
         <v>112</v>
       </c>
@@ -2956,7 +2973,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
         <v>112</v>
       </c>
@@ -2982,7 +2999,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
         <v>112</v>
       </c>
@@ -3008,7 +3025,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
         <v>112</v>
       </c>
@@ -3034,7 +3051,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
         <v>112</v>
       </c>
@@ -3060,7 +3077,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
         <v>112</v>
       </c>
@@ -3086,7 +3103,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
         <v>112</v>
       </c>
@@ -3112,7 +3129,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
         <v>112</v>
       </c>
@@ -3138,7 +3155,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
         <v>112</v>
       </c>
@@ -3164,7 +3181,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
         <v>112</v>
       </c>
@@ -3190,7 +3207,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
         <v>112</v>
       </c>
@@ -3216,7 +3233,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
         <v>112</v>
       </c>
@@ -3242,7 +3259,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
         <v>112</v>
       </c>
@@ -3268,7 +3285,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
         <v>112</v>
       </c>
@@ -3294,7 +3311,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
         <v>140</v>
       </c>
@@ -3317,7 +3334,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
         <v>140</v>
       </c>
@@ -3343,7 +3360,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
         <v>140</v>
       </c>
@@ -3369,7 +3386,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="89" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
         <v>140</v>
       </c>
@@ -3395,7 +3412,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
         <v>140</v>
       </c>
@@ -3421,7 +3438,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
         <v>140</v>
       </c>
@@ -3447,7 +3464,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="92" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
         <v>140</v>
       </c>
@@ -3473,7 +3490,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="93" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
         <v>140</v>
       </c>
@@ -3499,7 +3516,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="94" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
         <v>140</v>
       </c>
@@ -3525,7 +3542,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="95" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
         <v>140</v>
       </c>
@@ -3551,7 +3568,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="96" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
         <v>140</v>
       </c>
@@ -3577,7 +3594,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="97" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
         <v>140</v>
       </c>
@@ -3603,7 +3620,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="98" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
         <v>140</v>
       </c>
@@ -3629,7 +3646,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="99" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
         <v>140</v>
       </c>
@@ -3655,7 +3672,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="100" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
         <v>140</v>
       </c>
@@ -3681,7 +3698,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="101" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
         <v>140</v>
       </c>
@@ -3707,7 +3724,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="102" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
         <v>140</v>
       </c>
@@ -3733,7 +3750,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="103" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
         <v>140</v>
       </c>
@@ -3759,7 +3776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="104" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
         <v>140</v>
       </c>
@@ -3785,7 +3802,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="105" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
         <v>140</v>
       </c>
@@ -3811,7 +3828,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="106" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
         <v>140</v>
       </c>
@@ -3837,7 +3854,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="107" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
         <v>167</v>
       </c>
@@ -3860,7 +3877,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="108" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
         <v>167</v>
       </c>
@@ -3886,7 +3903,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="109" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
         <v>167</v>
       </c>
@@ -3912,7 +3929,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="110" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
         <v>167</v>
       </c>
@@ -3938,7 +3955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="111" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
         <v>167</v>
       </c>
@@ -3964,7 +3981,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="112" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
         <v>167</v>
       </c>
@@ -3990,7 +4007,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="113" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
         <v>167</v>
       </c>
@@ -4016,7 +4033,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="114" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
         <v>167</v>
       </c>
@@ -4042,7 +4059,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="115" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
         <v>167</v>
       </c>
@@ -4068,7 +4085,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="116" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
         <v>167</v>
       </c>
@@ -4094,7 +4111,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="117" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
         <v>167</v>
       </c>
@@ -4120,7 +4137,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="118" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
         <v>167</v>
       </c>
@@ -4146,7 +4163,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="119" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
         <v>167</v>
       </c>
@@ -4172,7 +4189,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="120" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
         <v>167</v>
       </c>
@@ -4198,7 +4215,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="121" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
         <v>167</v>
       </c>
@@ -4224,7 +4241,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="122" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
         <v>167</v>
       </c>
@@ -4250,7 +4267,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="123" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
         <v>167</v>
       </c>
@@ -4276,7 +4293,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="124" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
         <v>167</v>
       </c>
@@ -4302,7 +4319,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="125" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
         <v>167</v>
       </c>
@@ -4328,7 +4345,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="126" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
         <v>167</v>
       </c>
@@ -4354,7 +4371,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="127" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
         <v>167</v>
       </c>
@@ -4380,7 +4397,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="128" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
         <v>193</v>
       </c>
@@ -4403,7 +4420,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
         <v>193</v>
       </c>
@@ -4429,7 +4446,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
         <v>193</v>
       </c>
@@ -4455,7 +4472,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
         <v>193</v>
       </c>
@@ -4481,7 +4498,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
         <v>193</v>
       </c>
@@ -4507,7 +4524,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
         <v>193</v>
       </c>
@@ -4533,7 +4550,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
         <v>193</v>
       </c>
@@ -4559,7 +4576,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
         <v>193</v>
       </c>
@@ -4585,7 +4602,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="136" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="136" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
         <v>193</v>
       </c>
@@ -4611,7 +4628,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="137" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="137" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
         <v>193</v>
       </c>
@@ -4637,7 +4654,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="138" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="138" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
         <v>193</v>
       </c>
@@ -4663,7 +4680,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="139" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="139" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
         <v>193</v>
       </c>
@@ -4689,7 +4706,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="140" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="140" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
         <v>193</v>
       </c>
@@ -4715,7 +4732,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="141" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="141" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
         <v>193</v>
       </c>
@@ -4741,7 +4758,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="142" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="142" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
         <v>193</v>
       </c>
@@ -4767,7 +4784,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="143" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="143" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
         <v>193</v>
       </c>
@@ -4793,7 +4810,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="144" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="144" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
         <v>193</v>
       </c>
@@ -4819,7 +4836,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
         <v>193</v>
       </c>
@@ -4845,7 +4862,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
         <v>193</v>
       </c>
@@ -4871,7 +4888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
         <v>193</v>
       </c>
@@ -4897,7 +4914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
         <v>193</v>
       </c>
@@ -4920,6 +4937,29 @@
         <v>76</v>
       </c>
       <c r="H148" s="2" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A149" t="s">
+        <v>198</v>
+      </c>
+      <c r="B149" t="s">
+        <v>9</v>
+      </c>
+      <c r="C149" t="s">
+        <v>199</v>
+      </c>
+      <c r="D149">
+        <v>0</v>
+      </c>
+      <c r="E149" s="11" t="s">
+        <v>200</v>
+      </c>
+      <c r="F149" t="s">
+        <v>9</v>
+      </c>
+      <c r="H149" s="2" t="s">
         <v>12</v>
       </c>
     </row>

</xml_diff>